<commit_message>
Complemted day 7 part 2
</commit_message>
<xml_diff>
--- a/AdventOfCode2024Solutions/Day04/AOCd4p2.xlsx
+++ b/AdventOfCode2024Solutions/Day04/AOCd4p2.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f.madsen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f.madsen\source\repos\FMMadsen\AdventsOfCode\AdventOfCode2024Solutions\Day04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{143F5079-19F5-458E-B7FE-975FBF0A716C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1FC804-C4D0-4937-9AB9-CA18DA48F813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{783A48D8-EED0-4382-B7BB-4B625FC33AC8}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{783A48D8-EED0-4382-B7BB-4B625FC33AC8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Day4" sheetId="1" r:id="rId1"/>
+    <sheet name="Day7" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -534,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C5A1CC-0CE4-433C-9138-96431822105F}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -871,6 +872,76 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0648D66A-E1C5-40E0-801C-102C05BC892F}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>190</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+      <c r="C1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>72657447267</v>
+      </c>
+      <c r="B9">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>9</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>857</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{5fae8262-b78e-4366-8929-a5d6aac95320}" enabled="1" method="Standard" siteId="{cf36141c-ddd7-45a7-b073-111f66d0b30c}" contentBits="0" removed="0"/>

</xml_diff>